<commit_message>
update get neighbour feature and update c2dbdata
</commit_message>
<xml_diff>
--- a/find_spcaegroup/itemlist_formatted_1col.xlsx
+++ b/find_spcaegroup/itemlist_formatted_1col.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="246">
   <si>
     <t>material</t>
   </si>
@@ -28,7 +28,7 @@
     <t>Bi$_2$</t>
   </si>
   <si>
-    <t>None</t>
+    <t>e50c9fb190b0</t>
   </si>
   <si>
     <t>P-3m1 (164)</t>
@@ -46,12 +46,18 @@
     <t>P$_4$</t>
   </si>
   <si>
+    <t>276f0a298324</t>
+  </si>
+  <si>
     <t>Pmna (53)</t>
   </si>
   <si>
     <t>Sn$_2$</t>
   </si>
   <si>
+    <t>3deec82af6d4</t>
+  </si>
+  <si>
     <t>Al$_2$Cl$_6$</t>
   </si>
   <si>
@@ -392,9 +398,6 @@
   </si>
   <si>
     <t>e2a7fd3e05fc</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>PdO$_2$</t>
@@ -766,7 +769,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -806,7 +809,7 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -1120,8 +1123,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="22.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="21.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="22.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="21.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="4" width="14.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="4" width="21.576428571428572" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="4" width="21.576428571428572" customWidth="1" bestFit="1"/>
@@ -1129,7 +1132,7 @@
     <col min="7" max="7" style="4" width="18.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1144,7 +1147,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1159,7 +1162,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1174,27 +1177,27 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
@@ -1204,27 +1207,27 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1232,12 +1235,12 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -1245,12 +1248,12 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -1258,12 +1261,12 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -1271,12 +1274,12 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -1284,12 +1287,12 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -1297,12 +1300,12 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -1310,12 +1313,12 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -1323,12 +1326,12 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -1336,12 +1339,12 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1349,12 +1352,12 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1362,12 +1365,12 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -1375,12 +1378,12 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1388,12 +1391,12 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -1401,12 +1404,12 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -1414,12 +1417,12 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1427,12 +1430,12 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -1440,12 +1443,12 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -1453,12 +1456,12 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1466,12 +1469,12 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1479,12 +1482,12 @@
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1492,12 +1495,12 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -1505,12 +1508,12 @@
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1518,12 +1521,12 @@
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -1531,12 +1534,12 @@
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -1544,12 +1547,12 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -1557,12 +1560,12 @@
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -1570,12 +1573,12 @@
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -1583,12 +1586,12 @@
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -1596,12 +1599,12 @@
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -1609,12 +1612,12 @@
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
       <c r="A37" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -1622,12 +1625,12 @@
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
       <c r="A38" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -1635,12 +1638,12 @@
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
       <c r="A39" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -1648,12 +1651,12 @@
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
       <c r="A40" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -1661,12 +1664,12 @@
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
       <c r="A41" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -1674,12 +1677,12 @@
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
       <c r="A42" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -1687,12 +1690,12 @@
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
       <c r="A43" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -1700,12 +1703,12 @@
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
       <c r="A44" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -1713,12 +1716,12 @@
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
       <c r="A45" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -1726,12 +1729,12 @@
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
       <c r="A46" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -1739,12 +1742,12 @@
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
       <c r="A47" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -1754,10 +1757,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="17.25">
       <c r="A48" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -1767,10 +1770,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="17.25">
       <c r="A49" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -1780,10 +1783,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="17.25">
       <c r="A50" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -1793,10 +1796,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="17.25">
       <c r="A51" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -1806,10 +1809,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="17.25">
       <c r="A52" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -1819,10 +1822,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="17.25">
       <c r="A53" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -1832,10 +1835,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="17.25">
       <c r="A54" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -1845,10 +1848,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="17.25">
       <c r="A55" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -1858,10 +1861,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="17.25">
       <c r="A56" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -1871,10 +1874,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="17.25">
       <c r="A57" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -1884,10 +1887,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="17.25">
       <c r="A58" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -1897,10 +1900,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="17.25">
       <c r="A59" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -1910,10 +1913,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="17.25">
       <c r="A60" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -1923,10 +1926,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="17.25">
       <c r="A61" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -1936,10 +1939,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="17.25">
       <c r="A62" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -1949,10 +1952,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="17.25">
       <c r="A63" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -1962,895 +1965,777 @@
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="17.25">
       <c r="A64" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
-      <c r="G64" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G64" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="17.25">
       <c r="A65" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
-      <c r="G65" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G65" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="17.25">
       <c r="A66" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
-      <c r="G66" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G66" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="17.25">
       <c r="A67" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
-      <c r="G67" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G67" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="17.25">
       <c r="A68" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
-      <c r="G68" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G68" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="17.25">
       <c r="A69" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
-      <c r="G69" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G69" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="17.25">
       <c r="A70" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
-      <c r="G70" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G70" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="17.25">
       <c r="A71" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
-      <c r="G71" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G71" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="17.25">
       <c r="A72" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
-      <c r="G72" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G72" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="17.25">
       <c r="A73" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
-      <c r="G73" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G73" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="17.25">
       <c r="A74" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
-      <c r="G74" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G74" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="17.25">
       <c r="A75" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
-      <c r="G75" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G75" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="17.25">
       <c r="A76" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
-      <c r="G76" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G76" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="17.25">
       <c r="A77" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
-      <c r="G77" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G77" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="17.25">
       <c r="A78" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
-      <c r="G78" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G78" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="17.25">
       <c r="A79" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
-      <c r="G79" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G79" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="17.25">
       <c r="A80" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
-      <c r="G80" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G80" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="17.25">
       <c r="A81" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
-      <c r="G81" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G81" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="17.25">
       <c r="A82" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
-      <c r="G82" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G82" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="17.25">
       <c r="A83" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>
-      <c r="G83" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G83" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="17.25">
       <c r="A84" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>
-      <c r="G84" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G84" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="17.25">
       <c r="A85" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
-      <c r="G85" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G85" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="17.25">
       <c r="A86" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
-      <c r="G86" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G86" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="17.25">
       <c r="A87" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
-      <c r="G87" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G87" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="17.25">
       <c r="A88" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
-      <c r="G88" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G88" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="17.25">
       <c r="A89" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
-      <c r="G89" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G89" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="17.25">
       <c r="A90" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
-      <c r="G90" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G90" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="17.25">
       <c r="A91" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
-      <c r="G91" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G91" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="17.25">
       <c r="A92" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
       <c r="E92" s="2"/>
       <c r="F92" s="2"/>
-      <c r="G92" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G92" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="17.25">
       <c r="A93" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
       <c r="F93" s="2"/>
-      <c r="G93" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G93" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="17.25">
       <c r="A94" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
-      <c r="G94" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G94" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="17.25">
       <c r="A95" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
-      <c r="G95" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G95" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="17.25">
       <c r="A96" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
-      <c r="G96" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G96" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="17.25">
       <c r="A97" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C97" s="2"/>
       <c r="D97" s="2"/>
       <c r="E97" s="2"/>
       <c r="F97" s="2"/>
-      <c r="G97" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G97" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="17.25">
       <c r="A98" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
       <c r="F98" s="2"/>
-      <c r="G98" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G98" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="17.25">
       <c r="A99" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
       <c r="E99" s="2"/>
       <c r="F99" s="2"/>
-      <c r="G99" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G99" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="17.25">
       <c r="A100" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
       <c r="F100" s="2"/>
-      <c r="G100" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G100" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="17.25">
       <c r="A101" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
       <c r="F101" s="2"/>
-      <c r="G101" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G101" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="17.25">
       <c r="A102" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
-      <c r="G102" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G102" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="17.25">
       <c r="A103" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C103" s="2"/>
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
       <c r="F103" s="2"/>
-      <c r="G103" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G103" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="17.25">
       <c r="A104" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C104" s="2"/>
       <c r="D104" s="2"/>
       <c r="E104" s="2"/>
       <c r="F104" s="2"/>
-      <c r="G104" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G104" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="17.25">
       <c r="A105" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C105" s="2"/>
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
       <c r="F105" s="2"/>
-      <c r="G105" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G105" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="17.25">
       <c r="A106" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C106" s="2"/>
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
       <c r="F106" s="2"/>
-      <c r="G106" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G106" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="17.25">
       <c r="A107" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C107" s="2"/>
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
       <c r="F107" s="2"/>
-      <c r="G107" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G107" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="17.25">
       <c r="A108" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
       <c r="E108" s="2"/>
       <c r="F108" s="2"/>
-      <c r="G108" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G108" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="17.25">
       <c r="A109" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C109" s="2"/>
       <c r="D109" s="2"/>
       <c r="E109" s="2"/>
       <c r="F109" s="2"/>
-      <c r="G109" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G109" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="17.25">
       <c r="A110" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C110" s="2"/>
       <c r="D110" s="2"/>
       <c r="E110" s="2"/>
       <c r="F110" s="2"/>
-      <c r="G110" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G110" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="17.25">
       <c r="A111" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C111" s="2"/>
       <c r="D111" s="2"/>
       <c r="E111" s="2"/>
       <c r="F111" s="2"/>
-      <c r="G111" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G111" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="17.25">
       <c r="A112" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C112" s="2"/>
       <c r="D112" s="2"/>
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
-      <c r="G112" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G112" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="17.25">
       <c r="A113" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C113" s="2"/>
       <c r="D113" s="2"/>
       <c r="E113" s="2"/>
       <c r="F113" s="2"/>
-      <c r="G113" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G113" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="17.25">
       <c r="A114" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C114" s="2"/>
       <c r="D114" s="2"/>
       <c r="E114" s="2"/>
       <c r="F114" s="2"/>
-      <c r="G114" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G114" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="17.25">
       <c r="A115" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C115" s="2"/>
       <c r="D115" s="2"/>
       <c r="E115" s="2"/>
       <c r="F115" s="2"/>
-      <c r="G115" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G115" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="17.25">
       <c r="A116" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C116" s="2"/>
       <c r="D116" s="2"/>
       <c r="E116" s="2"/>
       <c r="F116" s="2"/>
-      <c r="G116" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G116" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="17.25">
       <c r="A117" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C117" s="2"/>
       <c r="D117" s="2"/>
       <c r="E117" s="2"/>
       <c r="F117" s="2"/>
-      <c r="G117" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G117" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="17.25">
       <c r="A118" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C118" s="2"/>
       <c r="D118" s="2"/>
       <c r="E118" s="2"/>
       <c r="F118" s="2"/>
-      <c r="G118" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G118" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="17.25">
       <c r="A119" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C119" s="2"/>
       <c r="D119" s="2"/>
       <c r="E119" s="2"/>
       <c r="F119" s="2"/>
-      <c r="G119" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G119" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="17.25">
       <c r="A120" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C120" s="2"/>
       <c r="D120" s="2"/>
       <c r="E120" s="2"/>
       <c r="F120" s="2"/>
-      <c r="G120" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G120" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="17.25">
       <c r="A121" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C121" s="2"/>
       <c r="D121" s="2"/>
       <c r="E121" s="2"/>
       <c r="F121" s="2"/>
-      <c r="G121" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G121" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="17.25">
       <c r="A122" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C122" s="2"/>
       <c r="D122" s="2"/>
       <c r="E122" s="2"/>
       <c r="F122" s="2"/>
-      <c r="G122" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="G122" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="17.25">
       <c r="A123" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C123" s="2"/>
       <c r="D123" s="2"/>
@@ -2860,10 +2745,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="17.25">
       <c r="A124" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C124" s="2"/>
       <c r="D124" s="2"/>
@@ -2873,10 +2758,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="17.25">
       <c r="A125" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C125" s="2"/>
       <c r="D125" s="2"/>

</xml_diff>